<commit_message>
update hccl excel report
</commit_message>
<xml_diff>
--- a/torch_distributed/hccl_report.xlsx
+++ b/torch_distributed/hccl_report.xlsx
@@ -453,10 +453,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="1" max="1"/>
     <col width="55" customWidth="1" min="2" max="2"/>
-    <col width="70" customWidth="1" min="3" max="3"/>
-    <col width="90" customWidth="1" min="4" max="4"/>
+    <col width="60" customWidth="1" min="3" max="3"/>
+    <col width="80" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -494,15 +494,13 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:459</t>
+          <t>torch_npu\contrib\transfer_to_npu.py:459</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:238  [['"]hccl['"]]
-  args_new[idx] = arg.replace('nccl', 'hccl')
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:243  [['"]hccl['"]]
-  kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
+          <t>L238 ["hccl"]: args_new[idx] = arg.replace('nccl', 'hccl')
+L243 ["hccl"]: kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
         </is>
       </c>
     </row>
@@ -519,59 +517,15 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207</t>
+          <t>torch_npu\__init__.py:207</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -588,59 +542,15 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195</t>
+          <t>torch_npu\__init__.py:195</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -657,15 +567,13 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:467</t>
+          <t>torch_npu\contrib\transfer_to_npu.py:467</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:238  [['"]hccl['"]]
-  args_new[idx] = arg.replace('nccl', 'hccl')
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:243  [['"]hccl['"]]
-  kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
+          <t>L238 ["hccl"]: args_new[idx] = arg.replace('nccl', 'hccl')
+L243 ["hccl"]: kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
         </is>
       </c>
     </row>
@@ -682,15 +590,13 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:464</t>
+          <t>torch_npu\contrib\transfer_to_npu.py:464</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:238  [['"]hccl['"]]
-  args_new[idx] = arg.replace('nccl', 'hccl')
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:243  [['"]hccl['"]]
-  kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
+          <t>L238 ["hccl"]: args_new[idx] = arg.replace('nccl', 'hccl')
+L243 ["hccl"]: kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
         </is>
       </c>
     </row>
@@ -707,15 +613,13 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:465</t>
+          <t>torch_npu\contrib\transfer_to_npu.py:465</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:238  [['"]hccl['"]]
-  args_new[idx] = arg.replace('nccl', 'hccl')
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:243  [['"]hccl['"]]
-  kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
+          <t>L238 ["hccl"]: args_new[idx] = arg.replace('nccl', 'hccl')
+L243 ["hccl"]: kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
         </is>
       </c>
     </row>
@@ -732,23 +636,17 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:667</t>
+          <t>torch_npu\distributed\distributed_c10d.py:667</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:127  [\bHCCL\b]
-  warnings.warn("HCCL doesn't support gather at the moment. Implemented with allgather instead.")
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:143  [\bHCCL\b]
-  warnings.warn("HCCL doesn't support gather at the moment. Implemented with allgather instead.")
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:222  [['"]hccl['"]]
-  return "hccl" in Backend.backend_list
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:255  [['"]hccl['"]]
-  if 'hccl' in backend:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:367  [['"]hccl['"]]
-  if backend == "hccl" or backend == "npu:hccl":
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:467  [\bHCCL\b]
-  elif Backend.HCCL in backend_config.get_device_backend_map().values():</t>
+          <t>L127 [HCCL]: warnings.warn("HCCL doesn't support gather at the moment. Implemented with allgather instead.")
+L222 ["hccl"]: return "hccl" in Backend.backend_list
+L255 ["hccl"]: if 'hccl' in backend:
+L367 ["hccl"]: if backend == "hccl" or backend == "npu:hccl":
+L467 [HCCL]: elif Backend.HCCL in backend_config.get_device_backend_map().values():
+... +1 more</t>
         </is>
       </c>
     </row>
@@ -765,59 +663,15 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196</t>
+          <t>torch_npu\__init__.py:196</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -834,59 +688,15 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198</t>
+          <t>torch_npu\__init__.py:198</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -903,59 +713,15 @@
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200</t>
+          <t>torch_npu\__init__.py:200</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -972,59 +738,15 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203</t>
+          <t>torch_npu\__init__.py:203</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -1041,15 +763,13 @@
       </c>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:460</t>
+          <t>torch_npu\contrib\transfer_to_npu.py:460</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:238  [['"]hccl['"]]
-  args_new[idx] = arg.replace('nccl', 'hccl')
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:243  [['"]hccl['"]]
-  kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
+          <t>L238 ["hccl"]: args_new[idx] = arg.replace('nccl', 'hccl')
+L243 ["hccl"]: kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
         </is>
       </c>
     </row>
@@ -1066,59 +786,15 @@
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:169</t>
+          <t>torch_npu\__init__.py:169</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -1135,59 +811,15 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197</t>
+          <t>torch_npu\__init__.py:197</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -1204,59 +836,15 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199</t>
+          <t>torch_npu\__init__.py:199</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -1273,15 +861,13 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:456</t>
+          <t>torch_npu\contrib\transfer_to_npu.py:456</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:238  [['"]hccl['"]]
-  args_new[idx] = arg.replace('nccl', 'hccl')
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:243  [['"]hccl['"]]
-  kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
+          <t>L238 ["hccl"]: args_new[idx] = arg.replace('nccl', 'hccl')
+L243 ["hccl"]: kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
         </is>
       </c>
     </row>
@@ -1298,59 +884,15 @@
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201</t>
+          <t>torch_npu\__init__.py:201</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -1367,15 +909,13 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:458</t>
+          <t>torch_npu\contrib\transfer_to_npu.py:458</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:238  [['"]hccl['"]]
-  args_new[idx] = arg.replace('nccl', 'hccl')
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:243  [['"]hccl['"]]
-  kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
+          <t>L238 ["hccl"]: args_new[idx] = arg.replace('nccl', 'hccl')
+L243 ["hccl"]: kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
         </is>
       </c>
     </row>
@@ -1392,59 +932,15 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204</t>
+          <t>torch_npu\__init__.py:204</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -1461,15 +957,13 @@
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:471</t>
+          <t>torch_npu\contrib\transfer_to_npu.py:471</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:238  [['"]hccl['"]]
-  args_new[idx] = arg.replace('nccl', 'hccl')
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\contrib\transfer_to_npu.py:243  [['"]hccl['"]]
-  kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
+          <t>L238 ["hccl"]: args_new[idx] = arg.replace('nccl', 'hccl')
+L243 ["hccl"]: kwargs['backend'] = backend.replace('nccl', 'hccl')</t>
         </is>
       </c>
     </row>
@@ -1486,59 +980,15 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202</t>
+          <t>torch_npu\__init__.py:202</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:82  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed.rpc
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:83  [\btorch_npu\.distributed\b]
-  import torch_npu.distributed._symmetric_memory
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:86  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.fsdp._add_fsdp_patch import _apply_fsdp_patch
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:87  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed.rpc.backend_registry import _rpc_backend_registry
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:97  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import ParallelStore
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:194  [\btorch_npu\.distributed\b]
-  torch._C._distributed_c10d._verify_params_across_processes = torch_npu.distributed._verify_params_across_processes
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:195  [\btorch_npu\.distributed\b]
-  torch.distributed.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:196  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.batch_isend_irecv = torch_npu.distributed.distributed_c10d._batch_isend_irecv
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:197  [\btorch_npu\.distributed\b]
-  torch.distributed.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:198  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather = torch_npu.distributed.distributed_c10d._gather
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:199  [\btorch_npu\.distributed\b]
-  torch.distributed.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:200  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.gather_object = torch_npu.distributed.distributed_c10d._gather_object
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:201  [\btorch_npu\.distributed\b]
-  torch.distributed.is_hccl_available = torch_npu.distributed.is_hccl_available
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:202  [\btorch_npu\.distributed\b]
-  torch.distributed.reinit_process_group = torch_npu.distributed.reinit_process_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:203  [\btorch_npu\.distributed\b]
-  torch.distributed.distributed_c10d.rendezvous = torch_npu.distributed.distributed_c10d._trigger_rendezvous_decorator(torch.distributed.distributed_c10d.rendezvous)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:204  [\btorch_npu\.distributed\b]
-  torch.distributed.launcher.api._get_addr_and_port = torch_npu.distributed.distributed_c10d._trigger__get_addr_and_port_decorator(torch.distributed.launcher.api._get_addr_and_port)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:206  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._hccl_get_sequence_number_for_group)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:207  [\btorch_npu\.distributed\b]
-  torch.distributed._symmetric_memory.enable_symm_mem_for_group = torch_npu.distributed._symmetric_memory._enable_symm_mem_for_group
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:247  [\bProcessGroupHCCL\b]
-  if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:248  [\bProcessGroupHCCL\b]
-  pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:253  [\bProcessGroupHCCL\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:260  [\btorch_npu\._C\._distributed_c10d\b]
-  return torch_npu._C._distributed_c10d.ProcessGroupLCCL(store, group_rank, group_size)
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:272  [['"]hccl['"]]
-  torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\__init__.py:288  [\btorch_npu\.distributed\b]
-  torch_npu.distributed.distributed_c10d._destructor_process_group()</t>
+          <t>L247 [ProcessGroupHCCL]: if pg_options is None or not isinstance(pg_options, torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options):
+L248 [ProcessGroupHCCL]: pg_options = torch_npu._C._distributed_c10d.ProcessGroupHCCL.Options()
+L253 [ProcessGroupHCCL]: return torch_npu._C._distributed_c10d.ProcessGroupHCCL(store, group_rank, group_size, pg_options)
+L272 ["hccl"]: torch.distributed.Backend.register_backend("hccl", lambda dist_backend_opts, pg_options:</t>
         </is>
       </c>
     </row>
@@ -1555,23 +1005,17 @@
       </c>
       <c r="C23" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:221</t>
+          <t>torch_npu\distributed\distributed_c10d.py:221</t>
         </is>
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:127  [\bHCCL\b]
-  warnings.warn("HCCL doesn't support gather at the moment. Implemented with allgather instead.")
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:143  [\bHCCL\b]
-  warnings.warn("HCCL doesn't support gather at the moment. Implemented with allgather instead.")
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:222  [['"]hccl['"]]
-  return "hccl" in Backend.backend_list
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:255  [['"]hccl['"]]
-  if 'hccl' in backend:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:367  [['"]hccl['"]]
-  if backend == "hccl" or backend == "npu:hccl":
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:467  [\bHCCL\b]
-  elif Backend.HCCL in backend_config.get_device_backend_map().values():</t>
+          <t>L127 [HCCL]: warnings.warn("HCCL doesn't support gather at the moment. Implemented with allgather instead.")
+L222 ["hccl"]: return "hccl" in Backend.backend_list
+L255 ["hccl"]: if 'hccl' in backend:
+L367 ["hccl"]: if backend == "hccl" or backend == "npu:hccl":
+L467 [HCCL]: elif Backend.HCCL in backend_config.get_device_backend_map().values():
+... +1 more</t>
         </is>
       </c>
     </row>
@@ -1588,23 +1032,17 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:243</t>
+          <t>torch_npu\distributed\distributed_c10d.py:243</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:127  [\bHCCL\b]
-  warnings.warn("HCCL doesn't support gather at the moment. Implemented with allgather instead.")
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:143  [\bHCCL\b]
-  warnings.warn("HCCL doesn't support gather at the moment. Implemented with allgather instead.")
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:222  [['"]hccl['"]]
-  return "hccl" in Backend.backend_list
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:255  [['"]hccl['"]]
-  if 'hccl' in backend:
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:367  [['"]hccl['"]]
-  if backend == "hccl" or backend == "npu:hccl":
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\distributed_c10d.py:467  [\bHCCL\b]
-  elif Backend.HCCL in backend_config.get_device_backend_map().values():</t>
+          <t>L127 [HCCL]: warnings.warn("HCCL doesn't support gather at the moment. Implemented with allgather instead.")
+L222 ["hccl"]: return "hccl" in Backend.backend_list
+L255 ["hccl"]: if 'hccl' in backend:
+L367 ["hccl"]: if backend == "hccl" or backend == "npu:hccl":
+L467 [HCCL]: elif Backend.HCCL in backend_config.get_device_backend_map().values():
+... +1 more</t>
         </is>
       </c>
     </row>
@@ -1621,17 +1059,14 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\__init__.py:9</t>
+          <t>torch_npu\distributed\__init__.py:9</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\__init__.py:22  [\btorch_npu\.distributed\b]
-  raise RuntimeError("Failed to initialize torch_npu.distributed" + dist_error(ErrCode.INTERNAL))
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\__init__.py:25  [\btorch_npu\._C\._distributed_c10d\b]
-  from torch_npu._C._distributed_c10d import (
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\__init__.py:32  [\btorch_npu\.distributed\b]
-  from torch_npu.distributed import rendezvous, fsdp, tensor</t>
+          <t>L22 [\btorch_npu\.distributed\b]: raise RuntimeError("Failed to initialize torch_npu.distributed" + dist_error(ErrCode.INTERNAL))
+L25 [\btorch_npu\._C\._distributed_c10d\b]: from torch_npu._C._distributed_c10d import (
+L32 [\btorch_npu\.distributed\b]: from torch_npu.distributed import rendezvous, fsdp, tensor</t>
         </is>
       </c>
     </row>
@@ -1648,25 +1083,17 @@
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:129</t>
+          <t>torch_npu\distributed\tensor\_matrix_ops.py:129</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:374  [\bhcom\b]
-  def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:376  [\bhcom\b]
-  # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:398  [\bhcom\b]
-  None,        # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:416  [\bhcom\b]
-  None,     # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:462  [\bhcom\b]
-  def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:464  [\bhcom\b]
-  # npu_mm_reduce_scatter_base(Tensor self, Tensor x2, str hcom, int world_size, *, str reduce_op='sum',
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:483  [\bhcom\b]
-  None,     # hcom</t>
+          <t>L374 [hcom]: def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
+L376 [hcom]: # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
+L398 [hcom]: None,        # hcom
+L416 [hcom]: None,     # hcom
+L462 [hcom]: def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
+... +2 more</t>
         </is>
       </c>
     </row>
@@ -1683,25 +1110,17 @@
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:60</t>
+          <t>torch_npu\distributed\tensor\_matrix_ops.py:60</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:374  [\bhcom\b]
-  def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:376  [\bhcom\b]
-  # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:398  [\bhcom\b]
-  None,        # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:416  [\bhcom\b]
-  None,     # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:462  [\bhcom\b]
-  def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:464  [\bhcom\b]
-  # npu_mm_reduce_scatter_base(Tensor self, Tensor x2, str hcom, int world_size, *, str reduce_op='sum',
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:483  [\bhcom\b]
-  None,     # hcom</t>
+          <t>L374 [hcom]: def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
+L376 [hcom]: # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
+L398 [hcom]: None,        # hcom
+L416 [hcom]: None,     # hcom
+L462 [hcom]: def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
+... +2 more</t>
         </is>
       </c>
     </row>
@@ -1718,25 +1137,17 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:374</t>
+          <t>torch_npu\distributed\tensor\_matrix_ops.py:374</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:374  [\bhcom\b]
-  def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:376  [\bhcom\b]
-  # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:398  [\bhcom\b]
-  None,        # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:416  [\bhcom\b]
-  None,     # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:462  [\bhcom\b]
-  def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:464  [\bhcom\b]
-  # npu_mm_reduce_scatter_base(Tensor self, Tensor x2, str hcom, int world_size, *, str reduce_op='sum',
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:483  [\bhcom\b]
-  None,     # hcom</t>
+          <t>L374 [hcom]: def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
+L376 [hcom]: # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
+L398 [hcom]: None,        # hcom
+L416 [hcom]: None,     # hcom
+L462 [hcom]: def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
+... +2 more</t>
         </is>
       </c>
     </row>
@@ -1753,25 +1164,17 @@
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:586</t>
+          <t>torch_npu\distributed\tensor\_matrix_ops.py:586</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:374  [\bhcom\b]
-  def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:376  [\bhcom\b]
-  # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:398  [\bhcom\b]
-  None,        # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:416  [\bhcom\b]
-  None,     # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:462  [\bhcom\b]
-  def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:464  [\bhcom\b]
-  # npu_mm_reduce_scatter_base(Tensor self, Tensor x2, str hcom, int world_size, *, str reduce_op='sum',
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:483  [\bhcom\b]
-  None,     # hcom</t>
+          <t>L374 [hcom]: def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
+L376 [hcom]: # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
+L398 [hcom]: None,        # hcom
+L416 [hcom]: None,     # hcom
+L462 [hcom]: def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
+... +2 more</t>
         </is>
       </c>
     </row>
@@ -1788,25 +1191,17 @@
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:524</t>
+          <t>torch_npu\distributed\tensor\_matrix_ops.py:524</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:374  [\bhcom\b]
-  def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:376  [\bhcom\b]
-  # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:398  [\bhcom\b]
-  None,        # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:416  [\bhcom\b]
-  None,     # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:462  [\bhcom\b]
-  def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:464  [\bhcom\b]
-  # npu_mm_reduce_scatter_base(Tensor self, Tensor x2, str hcom, int world_size, *, str reduce_op='sum',
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:483  [\bhcom\b]
-  None,     # hcom</t>
+          <t>L374 [hcom]: def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
+L376 [hcom]: # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
+L398 [hcom]: None,        # hcom
+L416 [hcom]: None,     # hcom
+L462 [hcom]: def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
+... +2 more</t>
         </is>
       </c>
     </row>
@@ -1823,25 +1218,17 @@
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:188</t>
+          <t>torch_npu\distributed\tensor\_matrix_ops.py:188</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:374  [\bhcom\b]
-  def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:376  [\bhcom\b]
-  # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:398  [\bhcom\b]
-  None,        # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:416  [\bhcom\b]
-  None,     # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:462  [\bhcom\b]
-  def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:464  [\bhcom\b]
-  # npu_mm_reduce_scatter_base(Tensor self, Tensor x2, str hcom, int world_size, *, str reduce_op='sum',
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:483  [\bhcom\b]
-  None,     # hcom</t>
+          <t>L374 [hcom]: def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
+L376 [hcom]: # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
+L398 [hcom]: None,        # hcom
+L416 [hcom]: None,     # hcom
+L462 [hcom]: def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
+... +2 more</t>
         </is>
       </c>
     </row>
@@ -1858,25 +1245,17 @@
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:462</t>
+          <t>torch_npu\distributed\tensor\_matrix_ops.py:462</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:374  [\bhcom\b]
-  def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:376  [\bhcom\b]
-  # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:398  [\bhcom\b]
-  None,        # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:416  [\bhcom\b]
-  None,     # hcom
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:462  [\bhcom\b]
-  def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:464  [\bhcom\b]
-  # npu_mm_reduce_scatter_base(Tensor self, Tensor x2, str hcom, int world_size, *, str reduce_op='sum',
-D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_matrix_ops.py:483  [\bhcom\b]
-  None,     # hcom</t>
+          <t>L374 [hcom]: def npu_all_gather_base_mm_strategy(x1, x2, hcom, world_size, bias=None, x1_scale=None, x2_scale=None, gather_index=0,
+L376 [hcom]: # npu_all_gather_base_mm(Tensor input, Tensor x2, str hcom, int world_size, *, Tensor? bias=None,
+L398 [hcom]: None,        # hcom
+L416 [hcom]: None,     # hcom
+L462 [hcom]: def npu_mm_reduce_scatter_base_strategy(x1, x2, hcom, world_size, reduce_op='sum', bias=None, x1_scale=None,
+... +2 more</t>
         </is>
       </c>
     </row>
@@ -1893,13 +1272,12 @@
       </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_math_ops.py:525</t>
+          <t>torch_npu\distributed\tensor\_math_ops.py:525</t>
         </is>
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_math_ops.py:0  [call-chain:custom_cross_entropy_loss_sharding -&gt; is_tensor_evenly_shardable -&gt; type]
-  (inferred via BFS)</t>
+          <t>custom_cross_entropy_loss_sharding -&gt; is_tensor_evenly_shardable -&gt; type</t>
         </is>
       </c>
     </row>
@@ -1916,13 +1294,12 @@
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_math_ops.py:658</t>
+          <t>torch_npu\distributed\tensor\_math_ops.py:658</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_math_ops.py:0  [call-chain:custom_npu_repeat_interleave_backward_int_strategy -&gt; is_tensor_evenly_shardable -&gt; type]
-  (inferred via BFS)</t>
+          <t>custom_npu_repeat_interleave_backward_int_strategy -&gt; is_tensor_evenly_shardable -&gt; type</t>
         </is>
       </c>
     </row>
@@ -1939,13 +1316,12 @@
       </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_math_ops.py:615</t>
+          <t>torch_npu\distributed\tensor\_math_ops.py:615</t>
         </is>
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_math_ops.py:0  [call-chain:custom_npu_repeat_interleave_self_int_strategy -&gt; is_tensor_evenly_shardable -&gt; type]
-  (inferred via BFS)</t>
+          <t>custom_npu_repeat_interleave_self_int_strategy -&gt; is_tensor_evenly_shardable -&gt; type</t>
         </is>
       </c>
     </row>
@@ -1962,13 +1338,12 @@
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_math_ops.py:498</t>
+          <t>torch_npu\distributed\tensor\_math_ops.py:498</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>D:\work\PyTorch\torchnpu\pytorch\torch_npu\distributed\tensor\_math_ops.py:0  [call-chain:is_tensor_evenly_shardable -&gt; type]
-  (inferred via BFS)</t>
+          <t>is_tensor_evenly_shardable -&gt; type</t>
         </is>
       </c>
     </row>

</xml_diff>